<commit_message>
Updated testdata.xlsx, updated AddCustomerTest for dp="dp2" logic
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SiloSix\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="17205" windowHeight="5370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>firstname</t>
   </si>
@@ -64,18 +64,6 @@
     <t>Rupee</t>
   </si>
   <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Ishita</t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Sehgal</t>
-  </si>
-  <si>
     <t>TCID</t>
   </si>
   <si>
@@ -92,12 +80,6 @@
   </si>
   <si>
     <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>runmode</t>
   </si>
 </sst>
 </file>
@@ -425,34 +407,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -462,15 +444,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,11 +465,8 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -499,60 +478,6 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -565,7 +490,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added logic for Runmode in testdata xls in listener onTestStart()
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>firstname</t>
   </si>
@@ -62,6 +62,18 @@
   </si>
   <si>
     <t>Rupee</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Ishita</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>Sehgal</t>
   </si>
   <si>
     <t>TCID</t>
@@ -407,34 +419,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -444,10 +456,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +489,48 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added onTestStart logic throw SkipException & onTestSkipped logic
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SiloSix\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\m6500A\w\w\git\jvm-selenium-ddt\src\test\resources\excel\_delete\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="17205" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="17205" windowHeight="5370"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>firstname</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -411,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +449,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -458,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>